<commit_message>
Added a find_best_fit function and the capability for the optimal_count_plan to use any fit function.
</commit_message>
<xml_diff>
--- a/GeneralNuclear/tests/testFiles/ExFoils.xlsx
+++ b/GeneralNuclear/tests/testFiles/ExFoils.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Dropbox\UCB\Research\ETAs\88Inch\Data\Simulated\Activation\50MeVTa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Dropbox\UCB\Computational_Tools\Scripts\Python\GeneralNuclear\tests\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>Radius [cm]</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>AlA</t>
+  </si>
+  <si>
+    <t>Relative Sigma</t>
+  </si>
+  <si>
+    <t>Detector to Foil [cm]</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,16 +537,18 @@
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
     <col min="4" max="4" width="9.109375" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="7.77734375" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="6"/>
-    <col min="16" max="16" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="7.77734375" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" style="6"/>
+    <col min="18" max="18" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -557,40 +565,46 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>22</v>
       </c>
@@ -606,44 +620,50 @@
       <c r="E2" s="9">
         <v>99.04</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G2" s="11">
+      <c r="I2" s="11">
         <v>1.4134600000000001E-6</v>
       </c>
-      <c r="H2" s="11">
+      <c r="J2" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I2" s="9">
+      <c r="K2" s="9">
         <v>2.5</v>
       </c>
-      <c r="J2" s="9">
+      <c r="L2" s="9">
         <v>0.1</v>
       </c>
-      <c r="K2" s="9">
+      <c r="M2" s="9">
         <v>6.49</v>
       </c>
-      <c r="L2" s="9">
+      <c r="N2" s="9">
         <v>91.224000000000004</v>
       </c>
-      <c r="M2" s="12">
+      <c r="O2" s="12">
         <v>0.51449999999999996</v>
       </c>
-      <c r="N2" s="13">
-        <f t="shared" ref="N2:N8" si="0">3.141592654*I2^2*J2</f>
+      <c r="P2" s="13">
+        <f t="shared" ref="P2:P8" si="0">3.141592654*K2^2*L2</f>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O2" s="14">
+      <c r="Q2" s="14">
         <f>78.41*3600</f>
         <v>282276</v>
       </c>
-      <c r="P2" s="15">
-        <f t="shared" ref="P2:P8" si="1">0.6931471806/O2</f>
+      <c r="R2" s="15">
+        <f t="shared" ref="R2:R8" si="1">0.6931471806/Q2</f>
         <v>2.4555654061981891E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
@@ -659,44 +679,50 @@
       <c r="E3" s="16">
         <v>81.7</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G3" s="17">
+      <c r="I3" s="17">
         <v>2.6853300000000001E-7</v>
       </c>
-      <c r="H3" s="11">
+      <c r="J3" s="11">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I3" s="9">
+      <c r="K3" s="9">
         <v>2.5</v>
       </c>
-      <c r="J3" s="9">
+      <c r="L3" s="9">
         <v>0.1</v>
       </c>
-      <c r="K3" s="13">
+      <c r="M3" s="13">
         <v>8.9079999999999995</v>
       </c>
-      <c r="L3" s="13">
+      <c r="N3" s="13">
         <v>58.693399999999997</v>
       </c>
-      <c r="M3" s="18">
+      <c r="O3" s="18">
         <v>0.68076899999999996</v>
       </c>
-      <c r="N3" s="13">
+      <c r="P3" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O3" s="19">
+      <c r="Q3" s="19">
         <f>35.6*3600</f>
         <v>128160</v>
       </c>
-      <c r="P3" s="15">
+      <c r="R3" s="15">
         <f t="shared" si="1"/>
         <v>5.4084517837078655E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -712,44 +738,50 @@
       <c r="E4" s="16">
         <v>99.45</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G4" s="17">
+      <c r="I4" s="17">
         <v>1.35264E-6</v>
       </c>
-      <c r="H4" s="17">
+      <c r="J4" s="17">
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="I4" s="9">
+      <c r="K4" s="9">
         <v>2.5</v>
       </c>
-      <c r="J4" s="9">
+      <c r="L4" s="9">
         <v>0.1</v>
       </c>
-      <c r="K4" s="8">
+      <c r="M4" s="8">
         <v>8.9079999999999995</v>
       </c>
-      <c r="L4" s="13">
+      <c r="N4" s="13">
         <v>58.693399999999997</v>
       </c>
-      <c r="M4" s="18">
+      <c r="O4" s="18">
         <v>0.68076899999999996</v>
       </c>
-      <c r="N4" s="13">
+      <c r="P4" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O4" s="19">
+      <c r="Q4" s="19">
         <f>70.86*24*3600</f>
         <v>6122304</v>
       </c>
-      <c r="P4" s="15">
+      <c r="R4" s="15">
         <f t="shared" si="1"/>
         <v>1.1321672046994073E-7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -765,44 +797,50 @@
       <c r="E5" s="9">
         <v>45.8</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="I5" s="11">
         <v>3.5202899999999998E-7</v>
       </c>
-      <c r="H5" s="17">
+      <c r="J5" s="17">
         <v>1.5E-3</v>
       </c>
-      <c r="I5" s="9">
+      <c r="K5" s="9">
         <v>2.5</v>
       </c>
-      <c r="J5" s="9">
+      <c r="L5" s="9">
         <v>0.1</v>
       </c>
-      <c r="K5" s="9">
+      <c r="M5" s="9">
         <v>7.31</v>
       </c>
-      <c r="L5" s="9">
+      <c r="N5" s="9">
         <v>114.818</v>
       </c>
-      <c r="M5" s="12">
+      <c r="O5" s="12">
         <v>0.95709999999999995</v>
       </c>
-      <c r="N5" s="13">
+      <c r="P5" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O5" s="14">
+      <c r="Q5" s="14">
         <f>4.5*3600</f>
         <v>16200</v>
       </c>
-      <c r="P5" s="15">
+      <c r="R5" s="15">
         <f t="shared" si="1"/>
         <v>4.2786863000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -818,44 +856,50 @@
       <c r="E6" s="9">
         <v>84.8</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="I6" s="11">
         <v>5.1103700000000003E-8</v>
       </c>
-      <c r="H6" s="11">
+      <c r="J6" s="11">
         <v>6.2300000000000001E-2</v>
       </c>
-      <c r="I6" s="9">
+      <c r="K6" s="9">
         <v>2.5</v>
       </c>
-      <c r="J6" s="9">
+      <c r="L6" s="9">
         <v>0.1</v>
       </c>
-      <c r="K6" s="9">
+      <c r="M6" s="9">
         <v>7.31</v>
       </c>
-      <c r="L6" s="9">
+      <c r="N6" s="9">
         <v>114.818</v>
       </c>
-      <c r="M6" s="12">
+      <c r="O6" s="12">
         <v>0.95709999999999995</v>
       </c>
-      <c r="N6" s="13">
+      <c r="P6" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O6" s="14">
+      <c r="Q6" s="14">
         <f>54.12*60</f>
         <v>3247.2</v>
       </c>
-      <c r="P6" s="15">
+      <c r="R6" s="15">
         <f t="shared" si="1"/>
         <v>2.134599595343681E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
@@ -871,44 +915,50 @@
       <c r="E7" s="16">
         <v>71.8</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G7" s="17">
+      <c r="I7" s="17">
         <v>2.4494200000000002E-7</v>
       </c>
-      <c r="H7" s="17">
+      <c r="J7" s="17">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="I7" s="9">
+      <c r="K7" s="9">
         <v>2.5</v>
       </c>
-      <c r="J7" s="9">
+      <c r="L7" s="9">
         <v>0.1</v>
       </c>
-      <c r="K7" s="9">
+      <c r="M7" s="9">
         <v>2.7</v>
       </c>
-      <c r="L7" s="9">
+      <c r="N7" s="9">
         <v>26.9815</v>
       </c>
-      <c r="M7" s="12">
+      <c r="O7" s="12">
         <v>1</v>
       </c>
-      <c r="N7" s="13">
+      <c r="P7" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O7" s="14">
+      <c r="Q7" s="14">
         <f>9.458*60</f>
         <v>567.48</v>
       </c>
-      <c r="P7" s="15">
+      <c r="R7" s="15">
         <f t="shared" si="1"/>
         <v>1.221447770141679E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
@@ -924,169 +974,175 @@
       <c r="E8" s="16">
         <v>99.99</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10">
         <v>4930000000</v>
       </c>
-      <c r="G8" s="17">
+      <c r="I8" s="17">
         <v>2.7114900000000001E-7</v>
       </c>
-      <c r="H8" s="17">
+      <c r="J8" s="17">
         <v>1E-3</v>
       </c>
-      <c r="I8" s="9">
+      <c r="K8" s="9">
         <v>2.5</v>
       </c>
-      <c r="J8" s="9">
+      <c r="L8" s="9">
         <v>0.1</v>
       </c>
-      <c r="K8" s="9">
+      <c r="M8" s="9">
         <v>2.7</v>
       </c>
-      <c r="L8" s="9">
+      <c r="N8" s="9">
         <v>26.9815</v>
       </c>
-      <c r="M8" s="12">
+      <c r="O8" s="12">
         <v>1</v>
       </c>
-      <c r="N8" s="13">
+      <c r="P8" s="13">
         <f t="shared" si="0"/>
         <v>1.9634954087500001</v>
       </c>
-      <c r="O8" s="14">
+      <c r="Q8" s="14">
         <f>15*3600</f>
         <v>54000</v>
       </c>
-      <c r="P8" s="15">
+      <c r="R8" s="15">
         <f t="shared" si="1"/>
         <v>1.28360589E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J10" s="2"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="2"/>
-      <c r="P10"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L10" s="2"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="2"/>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="10:11" x14ac:dyDescent="0.3">
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+    </row>
+    <row r="32" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+    </row>
+    <row r="40" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>